<commit_message>
Version 3.7.5 - add Diseño
</commit_message>
<xml_diff>
--- a/Imagenes/Map.xlsx
+++ b/Imagenes/Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>SabanaResearch</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>String name = "Monorriel"</t>
+  </si>
+  <si>
+    <t>String goal = ""Mejorar la movilidad de la ciudad</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -339,10 +342,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -354,10 +388,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,16 +424,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -390,58 +445,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3442,7 +3451,7 @@
   <dimension ref="B2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3454,7 +3463,7 @@
     <col min="14" max="14" width="9.7109375" customWidth="1"/>
     <col min="15" max="15" width="5.28515625" customWidth="1"/>
     <col min="16" max="16" width="16.7109375" customWidth="1"/>
-    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
@@ -3468,34 +3477,34 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="12"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="37"/>
+      <c r="Q3" s="31"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="20"/>
+      <c r="F4" s="14"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="35"/>
+      <c r="Q4" s="33"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="14"/>
       <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
@@ -3504,18 +3513,18 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="H6" s="27" t="s">
+      <c r="F6" s="16"/>
+      <c r="H6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="L6" s="38" t="s">
+      <c r="I6" s="20"/>
+      <c r="L6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="39"/>
+      <c r="M6" s="27"/>
       <c r="P6" s="5" t="s">
         <v>13</v>
       </c>
@@ -3523,22 +3532,22 @@
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="L7" s="40" t="s">
+      <c r="L7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="41"/>
-      <c r="P7" s="36" t="s">
+      <c r="M7" s="29"/>
+      <c r="P7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="37"/>
+      <c r="Q7" s="31"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="P8" s="34" t="s">
+      <c r="P8" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="35"/>
+      <c r="Q8" s="33"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H9" s="7"/>
@@ -3548,93 +3557,93 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="L10" s="38" t="s">
+      <c r="C10" s="12"/>
+      <c r="L10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="39"/>
+      <c r="M10" s="27"/>
       <c r="P10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="L11" s="40" t="s">
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="L11" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="41"/>
-      <c r="P11" s="36" t="s">
+      <c r="M11" s="29"/>
+      <c r="P11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="Q11" s="37"/>
+      <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P12" s="34" t="s">
+      <c r="P12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" s="35"/>
+      <c r="Q12" s="33"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="12"/>
       <c r="L13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="16"/>
-      <c r="L14" s="27" t="s">
+      <c r="I14" s="22"/>
+      <c r="L14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="28"/>
+      <c r="M14" s="20"/>
       <c r="P14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="P15" s="36" t="s">
+      <c r="I15" s="37"/>
+      <c r="P15" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="Q15" s="37"/>
+      <c r="Q15" s="31"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="20"/>
+      <c r="I16" s="14"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="P16" s="34" t="s">
+      <c r="P16" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="35"/>
+      <c r="Q16" s="33"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
+      <c r="I17" s="35"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
@@ -3650,11 +3659,11 @@
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
@@ -3664,106 +3673,110 @@
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="11"/>
+      <c r="F22" s="12"/>
       <c r="P22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="20"/>
+      <c r="F23" s="14"/>
       <c r="K23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P23" s="10" t="s">
+      <c r="P23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="Q23" s="11"/>
+      <c r="Q23" s="12"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="14"/>
       <c r="H24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="10" t="s">
+      <c r="K24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="11"/>
-      <c r="P24" s="15" t="s">
+      <c r="L24" s="12"/>
+      <c r="P24" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="Q24" s="16"/>
+      <c r="Q24" s="22"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="32"/>
-      <c r="H25" s="27" t="s">
+      <c r="F25" s="39"/>
+      <c r="H25" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="28"/>
-      <c r="K25" s="29" t="s">
+      <c r="I25" s="20"/>
+      <c r="K25" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L25" s="30"/>
-      <c r="P25" s="17" t="s">
+      <c r="L25" s="18"/>
+      <c r="P25" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Q25" s="18"/>
+      <c r="Q25" s="37"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="30"/>
+      <c r="F26" s="18"/>
       <c r="L26" s="8"/>
-      <c r="P26" s="19" t="s">
+      <c r="P26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="Q26" s="20"/>
+      <c r="Q26" s="14"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P27" s="21" t="s">
+      <c r="P27" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Q27" s="22"/>
+      <c r="Q27" s="14"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K28" s="10" t="s">
+      <c r="K28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="11"/>
+      <c r="L28" s="12"/>
+      <c r="P28" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q28" s="46"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="29" t="s">
+      <c r="K29" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L29" s="30"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="24"/>
+      <c r="F30" s="42"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="44"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K32" s="2" t="s">
@@ -3771,19 +3784,49 @@
       </c>
     </row>
     <row r="33" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K33" s="10" t="s">
+      <c r="K33" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L33" s="11"/>
+      <c r="L33" s="12"/>
     </row>
     <row r="34" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K34" s="29" t="s">
+      <c r="K34" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="30"/>
+      <c r="L34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="46">
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E6:F6"/>
@@ -3793,42 +3836,13 @@
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P11:Q11"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H25:I25"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="H15:I15"/>
     <mergeCell ref="K33:L33"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>